<commit_message>
update preload test doc ; update motion control module for change preload position.
</commit_message>
<xml_diff>
--- a/测试记录/测试需求表.xlsx
+++ b/测试记录/测试需求表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="功能测试" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="142">
   <si>
     <t>序号</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -144,10 +144,6 @@
   </si>
   <si>
     <t>位置超限</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>连续电流超过12A或者峰值电流超过16A时保护。</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -550,13 +546,57 @@
   <si>
     <t>通过改变电流环参数解决，需长期测试观察。</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>同一次穿戴条件下，运动1、2、5、10分钟后再次测试站立点。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>以自检速度的一半碰撞到机械限位时，电流出现持续30ms后驱动器进入保护状态。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试验证完成</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>连续电流超过12A或者峰值电流超过16A时保护。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>驱动器非使能状态下，拉动钢丝绳需要的力矩</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>不适用</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>驱动器非使能状态下，拉动钢丝绳需要，检测此时力传感器的数据。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>从静止状态下拉动需要15N-18N，拉动之后力矩很小无法计算得到。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>启动时间</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>记录开机启动到自检完成需要的时间。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>在未穿戴的状态下，启动需要2分13秒。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -622,6 +662,12 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -881,7 +927,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -912,6 +958,21 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1284,10 +1345,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1302,45 +1363,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="62.25" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="19"/>
-    </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="20"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22"/>
-    </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" ht="34.9" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="23"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26"/>
+      <c r="A1" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="24"/>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1" ht="20.25" x14ac:dyDescent="0.15">
+      <c r="A2" s="25"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="27"/>
+    </row>
+    <row r="3" spans="1:8" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.15">
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="31"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="28"/>
-    </row>
-    <row r="4" spans="1:8" s="7" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F3" s="30"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="33"/>
+    </row>
+    <row r="4" spans="1:8" s="7" customFormat="1" ht="20.25" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="30"/>
+      <c r="C4" s="35"/>
       <c r="D4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1358,10 +1419,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="112.5" x14ac:dyDescent="0.15">
-      <c r="A5" s="14">
+      <c r="A5" s="19">
         <v>1</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="16" t="s">
         <v>28</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -1374,153 +1435,155 @@
         <v>10</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:8" ht="56.25" x14ac:dyDescent="0.15">
-      <c r="A6" s="15"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>11</v>
-      </c>
+      <c r="A6" s="20"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="D6" s="8"/>
       <c r="E6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="8"/>
+        <v>140</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>141</v>
+      </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="1:8" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A7" s="15"/>
-      <c r="B7" s="12"/>
+    <row r="7" spans="1:8" ht="56.25" x14ac:dyDescent="0.15">
+      <c r="A7" s="20"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
     </row>
-    <row r="8" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="15"/>
-      <c r="B8" s="12"/>
+    <row r="8" spans="1:8" ht="37.5" x14ac:dyDescent="0.15">
+      <c r="A8" s="20"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="10" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
     </row>
-    <row r="9" spans="1:8" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A9" s="15"/>
-      <c r="B9" s="12"/>
+    <row r="9" spans="1:8" ht="18.75" x14ac:dyDescent="0.15">
+      <c r="A9" s="20"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="10" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
     </row>
-    <row r="10" spans="1:8" ht="56.25" x14ac:dyDescent="0.15">
-      <c r="A10" s="15"/>
-      <c r="B10" s="12"/>
+    <row r="10" spans="1:8" ht="37.5" x14ac:dyDescent="0.15">
+      <c r="A10" s="20"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="10" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" ht="56.25" x14ac:dyDescent="0.15">
-      <c r="A11" s="16"/>
-      <c r="B11" s="13"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="17"/>
       <c r="C11" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
     </row>
-    <row r="12" spans="1:8" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A12" s="14">
-        <v>2</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>42</v>
-      </c>
+    <row r="12" spans="1:8" ht="56.25" x14ac:dyDescent="0.15">
+      <c r="A12" s="21"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
     </row>
-    <row r="13" spans="1:8" ht="56.25" x14ac:dyDescent="0.15">
-      <c r="A13" s="15"/>
-      <c r="B13" s="12"/>
+    <row r="13" spans="1:8" ht="93.75" x14ac:dyDescent="0.15">
+      <c r="A13" s="19">
+        <v>2</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="C13" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="1:8" ht="56.25" x14ac:dyDescent="0.15">
+      <c r="A14" s="20"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-    </row>
-    <row r="14" spans="1:8" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A14" s="15"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="10" t="s">
-        <v>31</v>
-      </c>
       <c r="D14" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>113</v>
@@ -1531,55 +1594,73 @@
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="15"/>
-      <c r="B15" s="12"/>
+    <row r="15" spans="1:8" ht="37.5" x14ac:dyDescent="0.15">
+      <c r="A15" s="20"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="10" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="8"/>
+        <v>112</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>114</v>
+      </c>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
     </row>
-    <row r="16" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="16"/>
-      <c r="B16" s="13"/>
+    <row r="16" spans="1:8" ht="18.75" x14ac:dyDescent="0.15">
+      <c r="A16" s="20"/>
+      <c r="B16" s="17"/>
       <c r="C16" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="E16" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
     </row>
-    <row r="17" spans="1:8" ht="20.25" x14ac:dyDescent="0.15">
-      <c r="A17" s="3"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+    <row r="17" spans="1:8" ht="18.75" x14ac:dyDescent="0.15">
+      <c r="A17" s="21"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>40</v>
+      </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
     </row>
-    <row r="18" spans="1:8" ht="20.25" x14ac:dyDescent="0.15">
-      <c r="A18" s="3"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
+    <row r="18" spans="1:8" ht="75" x14ac:dyDescent="0.15">
+      <c r="A18" s="3">
+        <v>3</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>138</v>
+      </c>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
     </row>
@@ -1783,18 +1864,29 @@
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
     </row>
+    <row r="39" spans="1:8" ht="20.25" x14ac:dyDescent="0.15">
+      <c r="A39" s="3"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B5:B11"/>
-    <mergeCell ref="A5:A11"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="A12:A16"/>
+  <mergeCells count="11">
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="F3:H3"/>
-    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B5:B12"/>
+    <mergeCell ref="A5:A12"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="A13:A17"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1822,45 +1914,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="62.25" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="19"/>
+      <c r="A1" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" ht="20.25" x14ac:dyDescent="0.15">
-      <c r="A2" s="20"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:8" ht="22.5" x14ac:dyDescent="0.15">
-      <c r="A3" s="23"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="31"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="28"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:8" ht="20.25" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="30"/>
+      <c r="C4" s="35"/>
       <c r="D4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1917,10 +2009,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1936,53 +2028,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="62.25" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="19"/>
+      <c r="A1" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="24"/>
     </row>
     <row r="2" spans="1:9" ht="20.25" x14ac:dyDescent="0.15">
-      <c r="A2" s="20"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="22"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="27"/>
     </row>
     <row r="3" spans="1:9" ht="22.5" x14ac:dyDescent="0.15">
-      <c r="A3" s="23"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="31"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="28"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
     </row>
     <row r="4" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="30"/>
+      <c r="C4" s="35"/>
       <c r="D4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>3</v>
@@ -1991,7 +2083,7 @@
         <v>6</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>4</v>
@@ -2001,20 +2093,20 @@
       <c r="A5" s="3">
         <v>1</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>55</v>
+      <c r="B5" s="16" t="s">
+        <v>54</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I5" s="8"/>
     </row>
@@ -2022,41 +2114,41 @@
       <c r="A6" s="3">
         <v>2</v>
       </c>
-      <c r="B6" s="12"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>130</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="20.25" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>3</v>
       </c>
-      <c r="B7" s="12"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I7" s="8"/>
     </row>
@@ -2064,18 +2156,18 @@
       <c r="A8" s="3">
         <v>4</v>
       </c>
-      <c r="B8" s="12"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I8" s="8"/>
     </row>
@@ -2083,16 +2175,16 @@
       <c r="A9" s="3">
         <v>5</v>
       </c>
-      <c r="B9" s="12"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I9" s="8"/>
     </row>
@@ -2100,18 +2192,18 @@
       <c r="A10" s="3">
         <v>6</v>
       </c>
-      <c r="B10" s="12"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I10" s="8"/>
     </row>
@@ -2119,20 +2211,20 @@
       <c r="A11" s="3">
         <v>7</v>
       </c>
-      <c r="B11" s="12"/>
+      <c r="B11" s="17"/>
       <c r="C11" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I11" s="8"/>
     </row>
@@ -2140,20 +2232,20 @@
       <c r="A12" s="3">
         <v>8</v>
       </c>
-      <c r="B12" s="12"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I12" s="8"/>
     </row>
@@ -2161,20 +2253,20 @@
       <c r="A13" s="3">
         <v>9</v>
       </c>
-      <c r="B13" s="12"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" s="8" t="s">
         <v>118</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>119</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I13" s="8"/>
     </row>
@@ -2182,18 +2274,18 @@
       <c r="A14" s="3">
         <v>10</v>
       </c>
-      <c r="B14" s="12"/>
+      <c r="B14" s="17"/>
       <c r="C14" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I14" s="8"/>
     </row>
@@ -2201,18 +2293,18 @@
       <c r="A15" s="3">
         <v>11</v>
       </c>
-      <c r="B15" s="12"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I15" s="8"/>
     </row>
@@ -2220,18 +2312,18 @@
       <c r="A16" s="3">
         <v>12</v>
       </c>
-      <c r="B16" s="12"/>
+      <c r="B16" s="17"/>
       <c r="C16" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I16" s="8"/>
     </row>
@@ -2239,18 +2331,18 @@
       <c r="A17" s="3">
         <v>13</v>
       </c>
-      <c r="B17" s="12"/>
+      <c r="B17" s="17"/>
       <c r="C17" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I17" s="8"/>
     </row>
@@ -2258,18 +2350,18 @@
       <c r="A18" s="3">
         <v>14</v>
       </c>
-      <c r="B18" s="12"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I18" s="8"/>
     </row>
@@ -2277,18 +2369,18 @@
       <c r="A19" s="3">
         <v>15</v>
       </c>
-      <c r="B19" s="12"/>
+      <c r="B19" s="17"/>
       <c r="C19" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I19" s="8"/>
     </row>
@@ -2296,18 +2388,18 @@
       <c r="A20" s="3">
         <v>16</v>
       </c>
-      <c r="B20" s="12"/>
+      <c r="B20" s="17"/>
       <c r="C20" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I20" s="8"/>
     </row>
@@ -2315,18 +2407,18 @@
       <c r="A21" s="3">
         <v>17</v>
       </c>
-      <c r="B21" s="13"/>
+      <c r="B21" s="18"/>
       <c r="C21" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I21" s="8"/>
     </row>
@@ -2335,19 +2427,19 @@
         <v>18</v>
       </c>
       <c r="B22" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>74</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>75</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I22" s="8"/>
     </row>
@@ -2355,18 +2447,18 @@
       <c r="A23" s="3">
         <v>19</v>
       </c>
-      <c r="B23" s="11" t="s">
-        <v>99</v>
+      <c r="B23" s="16" t="s">
+        <v>98</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
@@ -2376,16 +2468,16 @@
       <c r="A24" s="3">
         <v>20</v>
       </c>
-      <c r="B24" s="12"/>
+      <c r="B24" s="17"/>
       <c r="C24" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
@@ -2395,9 +2487,9 @@
       <c r="A25" s="3">
         <v>21</v>
       </c>
-      <c r="B25" s="12"/>
+      <c r="B25" s="17"/>
       <c r="C25" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="8">
@@ -2412,9 +2504,9 @@
       <c r="A26" s="3">
         <v>22</v>
       </c>
-      <c r="B26" s="13"/>
+      <c r="B26" s="18"/>
       <c r="C26" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="8">
@@ -2429,22 +2521,22 @@
       <c r="A27" s="3">
         <v>23</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>121</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>122</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G27" s="8"/>
       <c r="H27" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I27" s="8"/>
     </row>
@@ -2452,31 +2544,35 @@
       <c r="A28" s="3">
         <v>24</v>
       </c>
-      <c r="B28" s="13"/>
+      <c r="B28" s="17"/>
       <c r="C28" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="F28" s="8" t="s">
         <v>127</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>128</v>
       </c>
       <c r="G28" s="8"/>
       <c r="H28" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I28" s="8"/>
     </row>
-    <row r="29" spans="1:9" ht="20.25" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9" ht="37.5" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
         <v>25</v>
       </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="10"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="11" t="s">
+        <v>122</v>
+      </c>
       <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
+      <c r="E29" s="8" t="s">
+        <v>131</v>
+      </c>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
@@ -2664,9 +2760,12 @@
       <c r="H43" s="8"/>
       <c r="I43" s="8"/>
     </row>
+    <row r="56" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B56" s="12"/>
+    </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B27:B29"/>
     <mergeCell ref="B23:B26"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:B21"/>
@@ -2686,8 +2785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2700,32 +2799,32 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B1" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="30"/>
+      <c r="C1" s="35"/>
       <c r="D1" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="56.25" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" s="32"/>
+      <c r="B2" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="37"/>
       <c r="D2" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>